<commit_message>
added Invalid scenarios test case
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DEPI-TASK-PAIR1\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95C46B2-76FD-431C-9E58-20676938857D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD777239-88C0-46C4-99FE-8C1500C587F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{012F7CE4-09FE-6C44-99A2-FD8570DDB851}"/>
   </bookViews>
@@ -89,9 +89,6 @@
     <t>Abc1</t>
   </si>
   <si>
-    <t xml:space="preserve">	user@test.com</t>
-  </si>
-  <si>
     <t>ShortPass</t>
   </si>
   <si>
@@ -135,6 +132,9 @@
   </si>
   <si>
     <t>!@#QWE123s</t>
+  </si>
+  <si>
+    <t>user@test.com</t>
   </si>
 </sst>
 </file>
@@ -545,7 +545,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -600,10 +600,10 @@
         <v>9</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="5" t="str">
-        <f t="shared" ref="D3:D9" si="0">C3</f>
+        <f t="shared" ref="D3:D8" si="0">C3</f>
         <v>P@ssw0rd!</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -625,7 +625,7 @@
         <v>Test@123</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -640,15 +640,15 @@
         <v xml:space="preserve">	Pass@123</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="1" t="s">
         <v>17</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>16</v>
@@ -658,35 +658,35 @@
         <v>Abc1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="D8" s="5" t="str">
         <f t="shared" si="0"/>
@@ -698,16 +698,16 @@
     </row>
     <row r="9" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>10</v>
@@ -767,6 +767,7 @@
     <hyperlink ref="B9" r:id="rId11" xr:uid="{AE32042A-2BBF-6B45-A79D-01093DFD8CA6}"/>
     <hyperlink ref="C3" r:id="rId12" xr:uid="{6655C62B-D43E-4878-B628-922C28288F23}"/>
     <hyperlink ref="D9" r:id="rId13" xr:uid="{F9B42D2B-CC99-4605-B48C-FEC934B089CE}"/>
+    <hyperlink ref="B6" r:id="rId14" xr:uid="{657A542C-536D-42B2-BD3C-B7A0AEA609EE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>